<commit_message>
update ops for external url
</commit_message>
<xml_diff>
--- a/CapStatement/DEQM_Capability_Statement_Aggregator_Client.xlsx
+++ b/CapStatement/DEQM_Capability_Statement_Aggregator_Client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\CapStatement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A899612-BF4F-45FC-AE04-C08461B7D46A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EA88F2-E2CC-4C82-9192-616F4E52380B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="555" windowWidth="28035" windowHeight="17445" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="765" yWindow="555" windowWidth="28035" windowHeight="17445" activeTab="3" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -337,13 +337,13 @@
     <t>SHOULD</t>
   </si>
   <si>
-    <t>The DaVinci DEQM Receiver Server **SHOULD** be capable of supporting the DEQM Summary MeasureReport Profile and  DEQM Individual MeasureReport Profile and all the DEQM and QI Core Profiles they reference.</t>
-  </si>
-  <si>
     <t>conf_MeasureReport</t>
   </si>
   <si>
     <t>aggregator-client</t>
+  </si>
+  <si>
+    <t>The DaVinci DEQM Aggregator Client **SHOULD** be capable of supporting the DEQM MeasureReport Profiles and all the DEQM and QI Core Profiles they reference.</t>
   </si>
 </sst>
 </file>
@@ -739,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15F3286-55C1-40D0-93FC-C97EF26956B8}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +762,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1067,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACB4CFA-AAEF-4FC6-A49B-107CEE80A317}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>97</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1217,7 +1217,7 @@
         <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>